<commit_message>
include unformatted data in table S1
</commit_message>
<xml_diff>
--- a/tables/table_S1.xlsx
+++ b/tables/table_S1.xlsx
@@ -1,18 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <workbookPr date1904="false"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="formatted" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="data" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="148">
   <si>
     <t xml:space="preserve">Species</t>
   </si>
@@ -23,6 +24,12 @@
     <t xml:space="preserve">Medium</t>
   </si>
   <si>
+    <t xml:space="preserve">ON_ratio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ON_ratio_se</t>
+  </si>
+  <si>
     <t xml:space="preserve">18eps / 15eps</t>
   </si>
   <si>
@@ -423,14 +430,44 @@
   </si>
   <si>
     <t xml:space="preserve">-11.7 +/- 0.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tracer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mu.1_hr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mu_se.1_hr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">eps15N.permil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">eps15N_se.permil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">eps18O.permil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">eps18O_se.permil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">no</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="166" formatCode="0.00"/>
+    <numFmt numFmtId="167" formatCode="0.00"/>
+  </numFmts>
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -443,6 +480,11 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <b/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -465,9 +507,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -754,20 +798,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="1"/>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="true"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <cols>
     <col min="1" max="1" width="19.71" hidden="0" customWidth="1"/>
     <col min="2" max="2" width="15.71" hidden="0" customWidth="1"/>
     <col min="3" max="3" width="15.71" hidden="0" customWidth="1"/>
-    <col min="4" max="4" width="13.71" hidden="0" customWidth="1"/>
-    <col min="5" max="5" width="13.71" hidden="0" customWidth="1"/>
+    <col min="4" max="4" width="8.71" hidden="0" customWidth="1"/>
+    <col min="5" max="5" width="11.71" hidden="0" customWidth="1"/>
     <col min="6" max="6" width="13.71" hidden="0" customWidth="1"/>
-    <col min="7" max="7" width="20.71" hidden="0" customWidth="1"/>
+    <col min="7" max="7" width="13.71" hidden="0" customWidth="1"/>
+    <col min="8" max="8" width="13.71" hidden="0" customWidth="1"/>
+    <col min="9" max="9" width="20.71" hidden="0" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -792,647 +838,2401 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" t="s">
         <v>11</v>
+      </c>
+      <c r="D2" s="2" t="n">
+        <v>0.605056749886199</v>
+      </c>
+      <c r="E2" s="2" t="n">
+        <v>0.0587262190457154</v>
       </c>
       <c r="F2" t="s">
         <v>12</v>
       </c>
       <c r="G2" t="s">
         <v>13</v>
+      </c>
+      <c r="H2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="3">
       <c r="A3"/>
       <c r="B3"/>
       <c r="C3"/>
-      <c r="D3"/>
-      <c r="E3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" t="s">
-        <v>15</v>
-      </c>
+      <c r="D3" s="2" t="n">
+        <v>0.605056749886199</v>
+      </c>
+      <c r="E3" s="2" t="n">
+        <v>0.0587262190457154</v>
+      </c>
+      <c r="F3"/>
       <c r="G3" t="s">
         <v>16</v>
+      </c>
+      <c r="H3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I3" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="4">
       <c r="A4"/>
       <c r="B4"/>
       <c r="C4"/>
-      <c r="D4"/>
-      <c r="E4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" t="s">
-        <v>18</v>
-      </c>
+      <c r="D4" s="2" t="n">
+        <v>0.605056749886199</v>
+      </c>
+      <c r="E4" s="2" t="n">
+        <v>0.0587262190457154</v>
+      </c>
+      <c r="F4"/>
       <c r="G4" t="s">
         <v>19</v>
       </c>
+      <c r="H4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I4" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E5" t="s">
-        <v>22</v>
+        <v>11</v>
+      </c>
+      <c r="D5" s="2" t="n">
+        <v>0.64183506129615</v>
+      </c>
+      <c r="E5" s="2" t="n">
+        <v>0.0352757479515451</v>
       </c>
       <c r="F5" t="s">
         <v>23</v>
       </c>
       <c r="G5" t="s">
         <v>24</v>
+      </c>
+      <c r="H5" t="s">
+        <v>25</v>
+      </c>
+      <c r="I5" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="6">
       <c r="A6"/>
       <c r="B6"/>
       <c r="C6"/>
-      <c r="D6"/>
-      <c r="E6" t="s">
-        <v>25</v>
-      </c>
-      <c r="F6" t="s">
-        <v>26</v>
-      </c>
+      <c r="D6" s="2" t="n">
+        <v>0.64183506129615</v>
+      </c>
+      <c r="E6" s="2" t="n">
+        <v>0.0352757479515451</v>
+      </c>
+      <c r="F6"/>
       <c r="G6" t="s">
         <v>27</v>
+      </c>
+      <c r="H6" t="s">
+        <v>28</v>
+      </c>
+      <c r="I6" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="7">
       <c r="A7"/>
       <c r="B7"/>
       <c r="C7" t="s">
-        <v>28</v>
-      </c>
-      <c r="D7"/>
-      <c r="E7" t="s">
-        <v>29</v>
-      </c>
-      <c r="F7" t="s">
         <v>30</v>
       </c>
-      <c r="G7"/>
+      <c r="D7" s="2" t="n">
+        <v>0.64183506129615</v>
+      </c>
+      <c r="E7" s="2" t="n">
+        <v>0.0352757479515451</v>
+      </c>
+      <c r="F7"/>
+      <c r="G7" t="s">
+        <v>31</v>
+      </c>
+      <c r="H7" t="s">
+        <v>32</v>
+      </c>
+      <c r="I7"/>
     </row>
     <row r="8">
       <c r="A8"/>
       <c r="B8"/>
       <c r="C8"/>
-      <c r="D8"/>
-      <c r="E8" t="s">
-        <v>31</v>
-      </c>
-      <c r="F8" t="s">
-        <v>32</v>
-      </c>
-      <c r="G8"/>
+      <c r="D8" s="2" t="n">
+        <v>0.64183506129615</v>
+      </c>
+      <c r="E8" s="2" t="n">
+        <v>0.0352757479515451</v>
+      </c>
+      <c r="F8"/>
+      <c r="G8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H8" t="s">
+        <v>34</v>
+      </c>
+      <c r="I8"/>
     </row>
     <row r="9">
       <c r="A9"/>
       <c r="B9"/>
       <c r="C9"/>
-      <c r="D9"/>
-      <c r="E9" t="s">
-        <v>33</v>
-      </c>
-      <c r="F9" t="s">
-        <v>34</v>
-      </c>
-      <c r="G9"/>
+      <c r="D9" s="2" t="n">
+        <v>0.64183506129615</v>
+      </c>
+      <c r="E9" s="2" t="n">
+        <v>0.0352757479515451</v>
+      </c>
+      <c r="F9"/>
+      <c r="G9" t="s">
+        <v>35</v>
+      </c>
+      <c r="H9" t="s">
+        <v>36</v>
+      </c>
+      <c r="I9"/>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B10" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C10" t="s">
-        <v>37</v>
-      </c>
-      <c r="D10" t="s">
-        <v>38</v>
-      </c>
-      <c r="E10" t="s">
         <v>39</v>
+      </c>
+      <c r="D10" s="2" t="n">
+        <v>0.629914490490416</v>
+      </c>
+      <c r="E10" s="2" t="n">
+        <v>0.0596188732139183</v>
       </c>
       <c r="F10" t="s">
         <v>40</v>
       </c>
-      <c r="G10"/>
+      <c r="G10" t="s">
+        <v>41</v>
+      </c>
+      <c r="H10" t="s">
+        <v>42</v>
+      </c>
+      <c r="I10"/>
     </row>
     <row r="11">
       <c r="A11"/>
       <c r="B11"/>
       <c r="C11"/>
-      <c r="D11"/>
-      <c r="E11" t="s">
-        <v>41</v>
-      </c>
-      <c r="F11" t="s">
-        <v>42</v>
-      </c>
-      <c r="G11"/>
+      <c r="D11" s="2" t="n">
+        <v>0.629914490490416</v>
+      </c>
+      <c r="E11" s="2" t="n">
+        <v>0.0596188732139183</v>
+      </c>
+      <c r="F11"/>
+      <c r="G11" t="s">
+        <v>43</v>
+      </c>
+      <c r="H11" t="s">
+        <v>44</v>
+      </c>
+      <c r="I11"/>
     </row>
     <row r="12">
       <c r="A12"/>
       <c r="B12"/>
       <c r="C12"/>
-      <c r="D12"/>
-      <c r="E12" t="s">
-        <v>43</v>
-      </c>
-      <c r="F12" t="s">
-        <v>44</v>
-      </c>
-      <c r="G12"/>
+      <c r="D12" s="2" t="n">
+        <v>0.629914490490416</v>
+      </c>
+      <c r="E12" s="2" t="n">
+        <v>0.0596188732139183</v>
+      </c>
+      <c r="F12"/>
+      <c r="G12" t="s">
+        <v>45</v>
+      </c>
+      <c r="H12" t="s">
+        <v>46</v>
+      </c>
+      <c r="I12"/>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B13" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C13" t="s">
-        <v>47</v>
-      </c>
-      <c r="D13" t="s">
-        <v>48</v>
-      </c>
-      <c r="E13" t="s">
         <v>49</v>
+      </c>
+      <c r="D13" s="2" t="n">
+        <v>0.965105401524031</v>
+      </c>
+      <c r="E13" s="2" t="n">
+        <v>0.0168010770398675</v>
       </c>
       <c r="F13" t="s">
         <v>50</v>
       </c>
       <c r="G13" t="s">
         <v>51</v>
+      </c>
+      <c r="H13" t="s">
+        <v>52</v>
+      </c>
+      <c r="I13" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="14">
       <c r="A14"/>
       <c r="B14"/>
       <c r="C14"/>
-      <c r="D14"/>
-      <c r="E14" t="s">
-        <v>52</v>
-      </c>
-      <c r="F14" t="s">
-        <v>53</v>
-      </c>
+      <c r="D14" s="2" t="n">
+        <v>0.965105401524031</v>
+      </c>
+      <c r="E14" s="2" t="n">
+        <v>0.0168010770398675</v>
+      </c>
+      <c r="F14"/>
       <c r="G14" t="s">
         <v>54</v>
+      </c>
+      <c r="H14" t="s">
+        <v>55</v>
+      </c>
+      <c r="I14" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="15">
       <c r="A15"/>
       <c r="B15"/>
       <c r="C15"/>
-      <c r="D15"/>
-      <c r="E15" t="s">
-        <v>55</v>
-      </c>
-      <c r="F15" t="s">
-        <v>56</v>
-      </c>
+      <c r="D15" s="2" t="n">
+        <v>0.965105401524031</v>
+      </c>
+      <c r="E15" s="2" t="n">
+        <v>0.0168010770398675</v>
+      </c>
+      <c r="F15"/>
       <c r="G15" t="s">
         <v>57</v>
+      </c>
+      <c r="H15" t="s">
+        <v>58</v>
+      </c>
+      <c r="I15" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="16">
       <c r="A16"/>
       <c r="B16"/>
       <c r="C16" t="s">
-        <v>58</v>
-      </c>
-      <c r="D16"/>
-      <c r="E16" t="s">
-        <v>59</v>
-      </c>
-      <c r="F16" t="s">
         <v>60</v>
       </c>
+      <c r="D16" s="2" t="n">
+        <v>0.965105401524031</v>
+      </c>
+      <c r="E16" s="2" t="n">
+        <v>0.0168010770398675</v>
+      </c>
+      <c r="F16"/>
       <c r="G16" t="s">
         <v>61</v>
+      </c>
+      <c r="H16" t="s">
+        <v>62</v>
+      </c>
+      <c r="I16" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="17">
       <c r="A17"/>
       <c r="B17"/>
       <c r="C17"/>
-      <c r="D17"/>
-      <c r="E17" t="s">
-        <v>62</v>
-      </c>
-      <c r="F17" t="s">
-        <v>63</v>
-      </c>
+      <c r="D17" s="2" t="n">
+        <v>0.965105401524031</v>
+      </c>
+      <c r="E17" s="2" t="n">
+        <v>0.0168010770398675</v>
+      </c>
+      <c r="F17"/>
       <c r="G17" t="s">
         <v>64</v>
+      </c>
+      <c r="H17" t="s">
+        <v>65</v>
+      </c>
+      <c r="I17" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="18">
       <c r="A18"/>
       <c r="B18"/>
       <c r="C18"/>
-      <c r="D18"/>
-      <c r="E18" t="s">
-        <v>65</v>
-      </c>
-      <c r="F18" t="s">
-        <v>66</v>
-      </c>
+      <c r="D18" s="2" t="n">
+        <v>0.965105401524031</v>
+      </c>
+      <c r="E18" s="2" t="n">
+        <v>0.0168010770398675</v>
+      </c>
+      <c r="F18"/>
       <c r="G18" t="s">
         <v>67</v>
+      </c>
+      <c r="H18" t="s">
+        <v>68</v>
+      </c>
+      <c r="I18" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="19">
       <c r="A19"/>
       <c r="B19"/>
       <c r="C19" t="s">
-        <v>68</v>
-      </c>
-      <c r="D19" t="s">
-        <v>69</v>
-      </c>
-      <c r="E19" t="s">
         <v>70</v>
+      </c>
+      <c r="D19" s="2" t="n">
+        <v>0.633008408485888</v>
+      </c>
+      <c r="E19" s="2" t="n">
+        <v>0.0222549617110416</v>
       </c>
       <c r="F19" t="s">
         <v>71</v>
       </c>
       <c r="G19" t="s">
         <v>72</v>
+      </c>
+      <c r="H19" t="s">
+        <v>73</v>
+      </c>
+      <c r="I19" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="20">
       <c r="A20"/>
       <c r="B20"/>
       <c r="C20"/>
-      <c r="D20"/>
-      <c r="E20" t="s">
-        <v>73</v>
-      </c>
-      <c r="F20" t="s">
-        <v>74</v>
-      </c>
+      <c r="D20" s="2" t="n">
+        <v>0.633008408485888</v>
+      </c>
+      <c r="E20" s="2" t="n">
+        <v>0.0222549617110416</v>
+      </c>
+      <c r="F20"/>
       <c r="G20" t="s">
         <v>75</v>
+      </c>
+      <c r="H20" t="s">
+        <v>76</v>
+      </c>
+      <c r="I20" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="21">
       <c r="A21"/>
       <c r="B21"/>
       <c r="C21"/>
-      <c r="D21"/>
-      <c r="E21" t="s">
-        <v>76</v>
-      </c>
-      <c r="F21" t="s">
-        <v>77</v>
-      </c>
+      <c r="D21" s="2" t="n">
+        <v>0.633008408485888</v>
+      </c>
+      <c r="E21" s="2" t="n">
+        <v>0.0222549617110416</v>
+      </c>
+      <c r="F21"/>
       <c r="G21" t="s">
         <v>78</v>
       </c>
+      <c r="H21" t="s">
+        <v>79</v>
+      </c>
+      <c r="I21" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B22" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C22" t="s">
-        <v>47</v>
-      </c>
-      <c r="D22" t="s">
-        <v>80</v>
-      </c>
-      <c r="E22" t="s">
-        <v>81</v>
+        <v>49</v>
+      </c>
+      <c r="D22" s="2" t="n">
+        <v>0.905853802645135</v>
+      </c>
+      <c r="E22" s="2" t="n">
+        <v>0.00934053653817344</v>
       </c>
       <c r="F22" t="s">
         <v>82</v>
       </c>
       <c r="G22" t="s">
-        <v>67</v>
+        <v>83</v>
+      </c>
+      <c r="H22" t="s">
+        <v>84</v>
+      </c>
+      <c r="I22" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="23">
       <c r="A23"/>
       <c r="B23"/>
       <c r="C23"/>
-      <c r="D23"/>
-      <c r="E23" t="s">
-        <v>83</v>
-      </c>
-      <c r="F23" t="s">
-        <v>84</v>
-      </c>
+      <c r="D23" s="2" t="n">
+        <v>0.905853802645135</v>
+      </c>
+      <c r="E23" s="2" t="n">
+        <v>0.00934053653817344</v>
+      </c>
+      <c r="F23"/>
       <c r="G23" t="s">
-        <v>67</v>
+        <v>85</v>
+      </c>
+      <c r="H23" t="s">
+        <v>86</v>
+      </c>
+      <c r="I23" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="24">
       <c r="A24"/>
       <c r="B24"/>
       <c r="C24" t="s">
-        <v>58</v>
-      </c>
-      <c r="D24"/>
-      <c r="E24" t="s">
-        <v>85</v>
-      </c>
-      <c r="F24" t="s">
-        <v>86</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="D24" s="2" t="n">
+        <v>0.905853802645135</v>
+      </c>
+      <c r="E24" s="2" t="n">
+        <v>0.00934053653817344</v>
+      </c>
+      <c r="F24"/>
       <c r="G24" t="s">
-        <v>67</v>
+        <v>87</v>
+      </c>
+      <c r="H24" t="s">
+        <v>88</v>
+      </c>
+      <c r="I24" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="25">
       <c r="A25"/>
       <c r="B25"/>
       <c r="C25"/>
-      <c r="D25"/>
-      <c r="E25" t="s">
-        <v>87</v>
-      </c>
-      <c r="F25" t="s">
-        <v>88</v>
-      </c>
+      <c r="D25" s="2" t="n">
+        <v>0.905853802645135</v>
+      </c>
+      <c r="E25" s="2" t="n">
+        <v>0.00934053653817344</v>
+      </c>
+      <c r="F25"/>
       <c r="G25" t="s">
-        <v>67</v>
+        <v>89</v>
+      </c>
+      <c r="H25" t="s">
+        <v>90</v>
+      </c>
+      <c r="I25" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="26">
       <c r="A26"/>
       <c r="B26"/>
       <c r="C26"/>
-      <c r="D26"/>
-      <c r="E26" t="s">
-        <v>89</v>
-      </c>
-      <c r="F26" t="s">
-        <v>90</v>
-      </c>
+      <c r="D26" s="2" t="n">
+        <v>0.905853802645135</v>
+      </c>
+      <c r="E26" s="2" t="n">
+        <v>0.00934053653817344</v>
+      </c>
+      <c r="F26"/>
       <c r="G26" t="s">
         <v>91</v>
+      </c>
+      <c r="H26" t="s">
+        <v>92</v>
+      </c>
+      <c r="I26" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="27">
       <c r="A27"/>
       <c r="B27"/>
       <c r="C27" t="s">
-        <v>68</v>
-      </c>
-      <c r="D27" t="s">
-        <v>92</v>
-      </c>
-      <c r="E27" t="s">
-        <v>93</v>
+        <v>70</v>
+      </c>
+      <c r="D27" s="2" t="n">
+        <v>0.847270404721274</v>
+      </c>
+      <c r="E27" s="2" t="n">
+        <v>0.0162504619702184</v>
       </c>
       <c r="F27" t="s">
         <v>94</v>
       </c>
       <c r="G27" t="s">
         <v>95</v>
+      </c>
+      <c r="H27" t="s">
+        <v>96</v>
+      </c>
+      <c r="I27" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="28">
       <c r="A28"/>
       <c r="B28"/>
       <c r="C28"/>
-      <c r="D28"/>
-      <c r="E28" t="s">
-        <v>96</v>
-      </c>
-      <c r="F28" t="s">
-        <v>97</v>
-      </c>
+      <c r="D28" s="2" t="n">
+        <v>0.847270404721274</v>
+      </c>
+      <c r="E28" s="2" t="n">
+        <v>0.0162504619702184</v>
+      </c>
+      <c r="F28"/>
       <c r="G28" t="s">
         <v>98</v>
+      </c>
+      <c r="H28" t="s">
+        <v>99</v>
+      </c>
+      <c r="I28" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="29">
       <c r="A29"/>
       <c r="B29"/>
       <c r="C29"/>
-      <c r="D29"/>
-      <c r="E29" t="s">
-        <v>99</v>
-      </c>
-      <c r="F29" t="s">
-        <v>100</v>
-      </c>
+      <c r="D29" s="2" t="n">
+        <v>0.847270404721274</v>
+      </c>
+      <c r="E29" s="2" t="n">
+        <v>0.0162504619702184</v>
+      </c>
+      <c r="F29"/>
       <c r="G29" t="s">
         <v>101</v>
       </c>
+      <c r="H29" t="s">
+        <v>102</v>
+      </c>
+      <c r="I29" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B30" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C30" t="s">
-        <v>47</v>
-      </c>
-      <c r="D30" t="s">
-        <v>103</v>
-      </c>
-      <c r="E30" t="s">
-        <v>104</v>
+        <v>49</v>
+      </c>
+      <c r="D30" s="2" t="n">
+        <v>0.487393975443699</v>
+      </c>
+      <c r="E30" s="2" t="n">
+        <v>0.00476070186935692</v>
       </c>
       <c r="F30" t="s">
         <v>105</v>
       </c>
       <c r="G30" t="s">
         <v>106</v>
+      </c>
+      <c r="H30" t="s">
+        <v>107</v>
+      </c>
+      <c r="I30" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="31">
       <c r="A31"/>
       <c r="B31"/>
       <c r="C31"/>
-      <c r="D31"/>
-      <c r="E31" t="s">
-        <v>107</v>
-      </c>
-      <c r="F31" t="s">
-        <v>108</v>
-      </c>
+      <c r="D31" s="2" t="n">
+        <v>0.487393975443699</v>
+      </c>
+      <c r="E31" s="2" t="n">
+        <v>0.00476070186935692</v>
+      </c>
+      <c r="F31"/>
       <c r="G31" t="s">
         <v>109</v>
+      </c>
+      <c r="H31" t="s">
+        <v>110</v>
+      </c>
+      <c r="I31" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="32">
       <c r="A32"/>
       <c r="B32"/>
       <c r="C32"/>
-      <c r="D32"/>
-      <c r="E32" t="s">
-        <v>110</v>
-      </c>
-      <c r="F32" t="s">
-        <v>111</v>
-      </c>
+      <c r="D32" s="2" t="n">
+        <v>0.487393975443699</v>
+      </c>
+      <c r="E32" s="2" t="n">
+        <v>0.00476070186935692</v>
+      </c>
+      <c r="F32"/>
       <c r="G32" t="s">
         <v>112</v>
+      </c>
+      <c r="H32" t="s">
+        <v>113</v>
+      </c>
+      <c r="I32" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="33">
       <c r="A33"/>
       <c r="B33"/>
       <c r="C33" t="s">
-        <v>58</v>
-      </c>
-      <c r="D33"/>
-      <c r="E33" t="s">
-        <v>113</v>
-      </c>
-      <c r="F33" t="s">
-        <v>114</v>
-      </c>
-      <c r="G33"/>
+        <v>60</v>
+      </c>
+      <c r="D33" s="2" t="n">
+        <v>0.487393975443699</v>
+      </c>
+      <c r="E33" s="2" t="n">
+        <v>0.00476070186935692</v>
+      </c>
+      <c r="F33"/>
+      <c r="G33" t="s">
+        <v>115</v>
+      </c>
+      <c r="H33" t="s">
+        <v>116</v>
+      </c>
+      <c r="I33"/>
     </row>
     <row r="34">
       <c r="A34"/>
       <c r="B34"/>
       <c r="C34"/>
-      <c r="D34"/>
-      <c r="E34" t="s">
-        <v>115</v>
-      </c>
-      <c r="F34" t="s">
-        <v>116</v>
-      </c>
-      <c r="G34"/>
+      <c r="D34" s="2" t="n">
+        <v>0.487393975443699</v>
+      </c>
+      <c r="E34" s="2" t="n">
+        <v>0.00476070186935692</v>
+      </c>
+      <c r="F34"/>
+      <c r="G34" t="s">
+        <v>117</v>
+      </c>
+      <c r="H34" t="s">
+        <v>118</v>
+      </c>
+      <c r="I34"/>
     </row>
     <row r="35">
       <c r="A35"/>
       <c r="B35"/>
       <c r="C35"/>
-      <c r="D35"/>
-      <c r="E35" t="s">
-        <v>117</v>
-      </c>
-      <c r="F35" t="s">
-        <v>118</v>
-      </c>
-      <c r="G35"/>
+      <c r="D35" s="2" t="n">
+        <v>0.487393975443699</v>
+      </c>
+      <c r="E35" s="2" t="n">
+        <v>0.00476070186935692</v>
+      </c>
+      <c r="F35"/>
+      <c r="G35" t="s">
+        <v>119</v>
+      </c>
+      <c r="H35" t="s">
+        <v>120</v>
+      </c>
+      <c r="I35"/>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B36" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C36" t="s">
-        <v>120</v>
-      </c>
-      <c r="D36" t="s">
-        <v>121</v>
-      </c>
-      <c r="E36" t="s">
         <v>122</v>
+      </c>
+      <c r="D36" s="2" t="n">
+        <v>0.915643588143238</v>
+      </c>
+      <c r="E36" s="2" t="n">
+        <v>0.00621994381504597</v>
       </c>
       <c r="F36" t="s">
         <v>123</v>
       </c>
-      <c r="G36"/>
+      <c r="G36" t="s">
+        <v>124</v>
+      </c>
+      <c r="H36" t="s">
+        <v>125</v>
+      </c>
+      <c r="I36"/>
     </row>
     <row r="37">
       <c r="A37"/>
       <c r="B37"/>
       <c r="C37"/>
-      <c r="D37"/>
-      <c r="E37" t="s">
-        <v>124</v>
-      </c>
-      <c r="F37" t="s">
-        <v>125</v>
-      </c>
+      <c r="D37" s="2" t="n">
+        <v>0.915643588143238</v>
+      </c>
+      <c r="E37" s="2" t="n">
+        <v>0.00621994381504597</v>
+      </c>
+      <c r="F37"/>
       <c r="G37" t="s">
         <v>126</v>
+      </c>
+      <c r="H37" t="s">
+        <v>127</v>
+      </c>
+      <c r="I37" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="38">
       <c r="A38"/>
       <c r="B38"/>
       <c r="C38"/>
-      <c r="D38"/>
-      <c r="E38" t="s">
-        <v>127</v>
-      </c>
-      <c r="F38" t="s">
-        <v>128</v>
-      </c>
+      <c r="D38" s="2" t="n">
+        <v>0.915643588143238</v>
+      </c>
+      <c r="E38" s="2" t="n">
+        <v>0.00621994381504597</v>
+      </c>
+      <c r="F38"/>
       <c r="G38" t="s">
         <v>129</v>
       </c>
+      <c r="H38" t="s">
+        <v>130</v>
+      </c>
+      <c r="I38" t="s">
+        <v>131</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="B39" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C39" t="s">
-        <v>131</v>
-      </c>
-      <c r="D39" t="s">
-        <v>132</v>
-      </c>
-      <c r="E39" t="s">
         <v>133</v>
+      </c>
+      <c r="D39" s="2" t="n">
+        <v>0.546725559293581</v>
+      </c>
+      <c r="E39" s="2" t="n">
+        <v>0.010561206245293</v>
       </c>
       <c r="F39" t="s">
         <v>134</v>
       </c>
-      <c r="G39"/>
+      <c r="G39" t="s">
+        <v>135</v>
+      </c>
+      <c r="H39" t="s">
+        <v>136</v>
+      </c>
+      <c r="I39"/>
     </row>
     <row r="40">
       <c r="A40"/>
       <c r="B40"/>
       <c r="C40"/>
-      <c r="D40"/>
-      <c r="E40" t="s">
-        <v>135</v>
-      </c>
-      <c r="F40" t="s">
-        <v>136</v>
-      </c>
-      <c r="G40"/>
+      <c r="D40" s="2" t="n">
+        <v>0.546725559293581</v>
+      </c>
+      <c r="E40" s="2" t="n">
+        <v>0.010561206245293</v>
+      </c>
+      <c r="F40"/>
+      <c r="G40" t="s">
+        <v>137</v>
+      </c>
+      <c r="H40" t="s">
+        <v>138</v>
+      </c>
+      <c r="I40"/>
+    </row>
+    <row r="41">
+      <c r="D41" s="2"/>
+      <c r="E41" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <cols>
+    <col min="1" max="1" width="19.71" hidden="0" customWidth="1"/>
+    <col min="2" max="2" width="15.71" hidden="0" customWidth="1"/>
+    <col min="3" max="3" width="8.71" hidden="0" customWidth="1"/>
+    <col min="4" max="4" width="6.71" hidden="0" customWidth="1"/>
+    <col min="5" max="5" width="7.71" hidden="0" customWidth="1"/>
+    <col min="6" max="6" width="10.71" hidden="0" customWidth="1"/>
+    <col min="7" max="7" width="13.71" hidden="0" customWidth="1"/>
+    <col min="8" max="8" width="16.71" hidden="0" customWidth="1"/>
+    <col min="9" max="9" width="13.71" hidden="0" customWidth="1"/>
+    <col min="10" max="10" width="16.71" hidden="0" customWidth="1"/>
+    <col min="11" max="11" width="8.71" hidden="0" customWidth="1"/>
+    <col min="12" max="12" width="11.71" hidden="0" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
+        <v>146</v>
+      </c>
+      <c r="E2" s="3" t="n">
+        <v>0.314775593584709</v>
+      </c>
+      <c r="F2" s="3" t="n">
+        <v>0.100856297507356</v>
+      </c>
+      <c r="G2" s="3" t="n">
+        <v>-15.3617593092816</v>
+      </c>
+      <c r="H2" s="3" t="n">
+        <v>1.55351559338663</v>
+      </c>
+      <c r="I2" s="3" t="n">
+        <v>-10.3925366408974</v>
+      </c>
+      <c r="J2" s="3" t="n">
+        <v>0.728718896446227</v>
+      </c>
+      <c r="K2" s="3" t="n">
+        <v>0.605056749886199</v>
+      </c>
+      <c r="L2" s="3" t="n">
+        <v>0.0587262190457154</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>146</v>
+      </c>
+      <c r="E3" s="3" t="n">
+        <v>0.241853779609417</v>
+      </c>
+      <c r="F3" s="3" t="n">
+        <v>0.0709249352555253</v>
+      </c>
+      <c r="G3" s="3" t="n">
+        <v>-13.6193905630674</v>
+      </c>
+      <c r="H3" s="3" t="n">
+        <v>1.96129242741741</v>
+      </c>
+      <c r="I3" s="3" t="n">
+        <v>-5.20029005454152</v>
+      </c>
+      <c r="J3" s="3" t="n">
+        <v>2.13169332093685</v>
+      </c>
+      <c r="K3" s="3" t="n">
+        <v>0.605056749886199</v>
+      </c>
+      <c r="L3" s="3" t="n">
+        <v>0.0587262190457154</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>146</v>
+      </c>
+      <c r="E4" s="3" t="n">
+        <v>0.244457031657793</v>
+      </c>
+      <c r="F4" s="3" t="n">
+        <v>0.0629997229592661</v>
+      </c>
+      <c r="G4" s="3" t="n">
+        <v>-11.7681117598092</v>
+      </c>
+      <c r="H4" s="3" t="n">
+        <v>2.067721220014</v>
+      </c>
+      <c r="I4" s="3" t="n">
+        <v>-8.05658038226191</v>
+      </c>
+      <c r="J4" s="3" t="n">
+        <v>0.747773090943202</v>
+      </c>
+      <c r="K4" s="3" t="n">
+        <v>0.605056749886199</v>
+      </c>
+      <c r="L4" s="3" t="n">
+        <v>0.0587262190457154</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" t="s">
+        <v>146</v>
+      </c>
+      <c r="E5" s="3" t="n">
+        <v>0.548981491727628</v>
+      </c>
+      <c r="F5" s="3" t="n">
+        <v>0.0508765803041468</v>
+      </c>
+      <c r="G5" s="3" t="n">
+        <v>-10.7973361009032</v>
+      </c>
+      <c r="H5" s="3" t="n">
+        <v>3.53349963801996</v>
+      </c>
+      <c r="I5" s="3" t="n">
+        <v>-9.70969111281823</v>
+      </c>
+      <c r="J5" s="3" t="n">
+        <v>2.07000136701354</v>
+      </c>
+      <c r="K5" s="3" t="n">
+        <v>0.64183506129615</v>
+      </c>
+      <c r="L5" s="3" t="n">
+        <v>0.0352757479515451</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" t="s">
+        <v>146</v>
+      </c>
+      <c r="E6" s="3" t="n">
+        <v>0.558490732107256</v>
+      </c>
+      <c r="F6" s="3" t="n">
+        <v>0.0401758091681455</v>
+      </c>
+      <c r="G6" s="3" t="n">
+        <v>-12.6425203972849</v>
+      </c>
+      <c r="H6" s="3" t="n">
+        <v>5.67247465114291</v>
+      </c>
+      <c r="I6" s="3" t="n">
+        <v>-9.26243398132257</v>
+      </c>
+      <c r="J6" s="3" t="n">
+        <v>4.07903491129841</v>
+      </c>
+      <c r="K6" s="3" t="n">
+        <v>0.64183506129615</v>
+      </c>
+      <c r="L6" s="3" t="n">
+        <v>0.0352757479515451</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" t="s">
+        <v>147</v>
+      </c>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3" t="n">
+        <v>-21.3270503393865</v>
+      </c>
+      <c r="H7" s="3" t="n">
+        <v>3.16908405986739</v>
+      </c>
+      <c r="I7" s="3" t="n">
+        <v>-11.3855015103082</v>
+      </c>
+      <c r="J7" s="3" t="n">
+        <v>2.80047280661526</v>
+      </c>
+      <c r="K7" s="3" t="n">
+        <v>0.64183506129615</v>
+      </c>
+      <c r="L7" s="3" t="n">
+        <v>0.0352757479515451</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" t="s">
+        <v>147</v>
+      </c>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3" t="n">
+        <v>-20.9527016779056</v>
+      </c>
+      <c r="H8" s="3" t="n">
+        <v>3.57061692050139</v>
+      </c>
+      <c r="I8" s="3" t="n">
+        <v>-13.0587776042771</v>
+      </c>
+      <c r="J8" s="3" t="n">
+        <v>2.17739929659694</v>
+      </c>
+      <c r="K8" s="3" t="n">
+        <v>0.64183506129615</v>
+      </c>
+      <c r="L8" s="3" t="n">
+        <v>0.0352757479515451</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" t="s">
+        <v>147</v>
+      </c>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3" t="n">
+        <v>-10.9114964599315</v>
+      </c>
+      <c r="H9" s="3" t="n">
+        <v>4.63237661125512</v>
+      </c>
+      <c r="I9" s="3" t="n">
+        <v>-6.27910952056183</v>
+      </c>
+      <c r="J9" s="3" t="n">
+        <v>2.55059732298709</v>
+      </c>
+      <c r="K9" s="3" t="n">
+        <v>0.64183506129615</v>
+      </c>
+      <c r="L9" s="3" t="n">
+        <v>0.0352757479515451</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" t="s">
+        <v>146</v>
+      </c>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3" t="n">
+        <v>-22.014542928056</v>
+      </c>
+      <c r="H10" s="3" t="n">
+        <v>0.380100443879606</v>
+      </c>
+      <c r="I10" s="3" t="n">
+        <v>-13.8740833359191</v>
+      </c>
+      <c r="J10" s="3" t="n">
+        <v>3.0993270850094</v>
+      </c>
+      <c r="K10" s="3" t="n">
+        <v>0.629914490490416</v>
+      </c>
+      <c r="L10" s="3" t="n">
+        <v>0.0596188732139183</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" t="s">
+        <v>146</v>
+      </c>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3" t="n">
+        <v>-24.0692190417925</v>
+      </c>
+      <c r="H11" s="3" t="n">
+        <v>1.17339529956727</v>
+      </c>
+      <c r="I11" s="3" t="n">
+        <v>-15.2196118396256</v>
+      </c>
+      <c r="J11" s="3" t="n">
+        <v>2.38416247546109</v>
+      </c>
+      <c r="K11" s="3" t="n">
+        <v>0.629914490490416</v>
+      </c>
+      <c r="L11" s="3" t="n">
+        <v>0.0596188732139183</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" t="s">
+        <v>146</v>
+      </c>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3" t="n">
+        <v>-24.7988315734454</v>
+      </c>
+      <c r="H12" s="3" t="n">
+        <v>1.37203184413252</v>
+      </c>
+      <c r="I12" s="3" t="n">
+        <v>-15.8128470860815</v>
+      </c>
+      <c r="J12" s="3" t="n">
+        <v>3.32250508450005</v>
+      </c>
+      <c r="K12" s="3" t="n">
+        <v>0.629914490490416</v>
+      </c>
+      <c r="L12" s="3" t="n">
+        <v>0.0596188732139183</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>47</v>
+      </c>
+      <c r="B13" t="s">
+        <v>48</v>
+      </c>
+      <c r="C13" t="s">
+        <v>49</v>
+      </c>
+      <c r="D13" t="s">
+        <v>146</v>
+      </c>
+      <c r="E13" s="3" t="n">
+        <v>0.110031617970778</v>
+      </c>
+      <c r="F13" s="3" t="n">
+        <v>0.0369723982718034</v>
+      </c>
+      <c r="G13" s="3" t="n">
+        <v>-28.4238193537088</v>
+      </c>
+      <c r="H13" s="3" t="n">
+        <v>1.18361964036476</v>
+      </c>
+      <c r="I13" s="3" t="n">
+        <v>-26.1815342296879</v>
+      </c>
+      <c r="J13" s="3" t="n">
+        <v>1.42811164259897</v>
+      </c>
+      <c r="K13" s="3" t="n">
+        <v>0.965105401524031</v>
+      </c>
+      <c r="L13" s="3" t="n">
+        <v>0.0168010770398675</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>47</v>
+      </c>
+      <c r="B14" t="s">
+        <v>48</v>
+      </c>
+      <c r="C14" t="s">
+        <v>49</v>
+      </c>
+      <c r="D14" t="s">
+        <v>146</v>
+      </c>
+      <c r="E14" s="3" t="n">
+        <v>0.0971778210293567</v>
+      </c>
+      <c r="F14" s="3" t="n">
+        <v>0.0449096225653793</v>
+      </c>
+      <c r="G14" s="3" t="n">
+        <v>-27.7462954448834</v>
+      </c>
+      <c r="H14" s="3" t="n">
+        <v>0.471228851862108</v>
+      </c>
+      <c r="I14" s="3" t="n">
+        <v>-25.7678223811416</v>
+      </c>
+      <c r="J14" s="3" t="n">
+        <v>0.939967733324501</v>
+      </c>
+      <c r="K14" s="3" t="n">
+        <v>0.965105401524031</v>
+      </c>
+      <c r="L14" s="3" t="n">
+        <v>0.0168010770398675</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>47</v>
+      </c>
+      <c r="B15" t="s">
+        <v>48</v>
+      </c>
+      <c r="C15" t="s">
+        <v>49</v>
+      </c>
+      <c r="D15" t="s">
+        <v>146</v>
+      </c>
+      <c r="E15" s="3" t="n">
+        <v>0.113805102030626</v>
+      </c>
+      <c r="F15" s="3" t="n">
+        <v>0.0343260700684518</v>
+      </c>
+      <c r="G15" s="3" t="n">
+        <v>-28.5092508577638</v>
+      </c>
+      <c r="H15" s="3" t="n">
+        <v>0.593910851455606</v>
+      </c>
+      <c r="I15" s="3" t="n">
+        <v>-26.7718103732458</v>
+      </c>
+      <c r="J15" s="3" t="n">
+        <v>0.830438717970516</v>
+      </c>
+      <c r="K15" s="3" t="n">
+        <v>0.965105401524031</v>
+      </c>
+      <c r="L15" s="3" t="n">
+        <v>0.0168010770398675</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16" t="s">
+        <v>48</v>
+      </c>
+      <c r="C16" t="s">
+        <v>49</v>
+      </c>
+      <c r="D16" t="s">
+        <v>147</v>
+      </c>
+      <c r="E16" s="3" t="n">
+        <v>0.0532803574971597</v>
+      </c>
+      <c r="F16" s="3" t="n">
+        <v>0.0199924739690356</v>
+      </c>
+      <c r="G16" s="3" t="n">
+        <v>-22.6125338452201</v>
+      </c>
+      <c r="H16" s="3" t="n">
+        <v>2.41482181245862</v>
+      </c>
+      <c r="I16" s="3" t="n">
+        <v>-21.8260458903655</v>
+      </c>
+      <c r="J16" s="3" t="n">
+        <v>2.21882369098446</v>
+      </c>
+      <c r="K16" s="3" t="n">
+        <v>0.965105401524031</v>
+      </c>
+      <c r="L16" s="3" t="n">
+        <v>0.0168010770398675</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>47</v>
+      </c>
+      <c r="B17" t="s">
+        <v>48</v>
+      </c>
+      <c r="C17" t="s">
+        <v>49</v>
+      </c>
+      <c r="D17" t="s">
+        <v>147</v>
+      </c>
+      <c r="E17" s="3" t="n">
+        <v>0.0618306962480331</v>
+      </c>
+      <c r="F17" s="3" t="n">
+        <v>0.0198123407332675</v>
+      </c>
+      <c r="G17" s="3" t="n">
+        <v>-26.7851321077069</v>
+      </c>
+      <c r="H17" s="3" t="n">
+        <v>0.406929916130505</v>
+      </c>
+      <c r="I17" s="3" t="n">
+        <v>-24.508470537939</v>
+      </c>
+      <c r="J17" s="3" t="n">
+        <v>1.29049700646206</v>
+      </c>
+      <c r="K17" s="3" t="n">
+        <v>0.965105401524031</v>
+      </c>
+      <c r="L17" s="3" t="n">
+        <v>0.0168010770398675</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>47</v>
+      </c>
+      <c r="B18" t="s">
+        <v>48</v>
+      </c>
+      <c r="C18" t="s">
+        <v>49</v>
+      </c>
+      <c r="D18" t="s">
+        <v>147</v>
+      </c>
+      <c r="E18" s="3" t="n">
+        <v>0.094221421611188</v>
+      </c>
+      <c r="F18" s="3" t="n">
+        <v>0.0129713372243432</v>
+      </c>
+      <c r="G18" s="3" t="n">
+        <v>-23.4980000522594</v>
+      </c>
+      <c r="H18" s="3" t="n">
+        <v>2.15925235584067</v>
+      </c>
+      <c r="I18" s="3" t="n">
+        <v>-24.5335525404303</v>
+      </c>
+      <c r="J18" s="3" t="n">
+        <v>1.41679345097281</v>
+      </c>
+      <c r="K18" s="3" t="n">
+        <v>0.965105401524031</v>
+      </c>
+      <c r="L18" s="3" t="n">
+        <v>0.0168010770398675</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>47</v>
+      </c>
+      <c r="B19" t="s">
+        <v>48</v>
+      </c>
+      <c r="C19" t="s">
+        <v>70</v>
+      </c>
+      <c r="D19" t="s">
+        <v>146</v>
+      </c>
+      <c r="E19" s="3" t="n">
+        <v>0.121721169199298</v>
+      </c>
+      <c r="F19" s="3" t="n">
+        <v>0.0323416386456169</v>
+      </c>
+      <c r="G19" s="3" t="n">
+        <v>-23.3788599457968</v>
+      </c>
+      <c r="H19" s="3" t="n">
+        <v>0.949980618243649</v>
+      </c>
+      <c r="I19" s="3" t="n">
+        <v>-15.298039598923</v>
+      </c>
+      <c r="J19" s="3" t="n">
+        <v>1.23418921575289</v>
+      </c>
+      <c r="K19" s="3" t="n">
+        <v>0.633008408485888</v>
+      </c>
+      <c r="L19" s="3" t="n">
+        <v>0.0222549617110416</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>47</v>
+      </c>
+      <c r="B20" t="s">
+        <v>48</v>
+      </c>
+      <c r="C20" t="s">
+        <v>70</v>
+      </c>
+      <c r="D20" t="s">
+        <v>146</v>
+      </c>
+      <c r="E20" s="3" t="n">
+        <v>0.139615349826987</v>
+      </c>
+      <c r="F20" s="3" t="n">
+        <v>0.0332302860329463</v>
+      </c>
+      <c r="G20" s="3" t="n">
+        <v>-22.5184171499221</v>
+      </c>
+      <c r="H20" s="3" t="n">
+        <v>0.96301342960951</v>
+      </c>
+      <c r="I20" s="3" t="n">
+        <v>-14.3295016860481</v>
+      </c>
+      <c r="J20" s="3" t="n">
+        <v>1.84694376011389</v>
+      </c>
+      <c r="K20" s="3" t="n">
+        <v>0.633008408485888</v>
+      </c>
+      <c r="L20" s="3" t="n">
+        <v>0.0222549617110416</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>47</v>
+      </c>
+      <c r="B21" t="s">
+        <v>48</v>
+      </c>
+      <c r="C21" t="s">
+        <v>70</v>
+      </c>
+      <c r="D21" t="s">
+        <v>146</v>
+      </c>
+      <c r="E21" s="3" t="n">
+        <v>0.106005131546667</v>
+      </c>
+      <c r="F21" s="3" t="n">
+        <v>0.00350606447502223</v>
+      </c>
+      <c r="G21" s="3" t="n">
+        <v>-22.9549302405719</v>
+      </c>
+      <c r="H21" s="3" t="n">
+        <v>0.371731181844035</v>
+      </c>
+      <c r="I21" s="3" t="n">
+        <v>-14.0657606630624</v>
+      </c>
+      <c r="J21" s="3" t="n">
+        <v>1.2061510881592</v>
+      </c>
+      <c r="K21" s="3" t="n">
+        <v>0.633008408485888</v>
+      </c>
+      <c r="L21" s="3" t="n">
+        <v>0.0222549617110416</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>81</v>
+      </c>
+      <c r="B22" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22" t="s">
+        <v>49</v>
+      </c>
+      <c r="D22" t="s">
+        <v>146</v>
+      </c>
+      <c r="E22" s="3" t="n">
+        <v>0.0858854392763567</v>
+      </c>
+      <c r="F22" s="3" t="n">
+        <v>0.00762625056965242</v>
+      </c>
+      <c r="G22" s="3" t="n">
+        <v>-24.9103014445467</v>
+      </c>
+      <c r="H22" s="3" t="n">
+        <v>2.01947816927322</v>
+      </c>
+      <c r="I22" s="3" t="n">
+        <v>-22.7019803289009</v>
+      </c>
+      <c r="J22" s="3" t="n">
+        <v>1.82728932136806</v>
+      </c>
+      <c r="K22" s="3" t="n">
+        <v>0.905853802645135</v>
+      </c>
+      <c r="L22" s="3" t="n">
+        <v>0.00934053653817344</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>81</v>
+      </c>
+      <c r="B23" t="s">
+        <v>10</v>
+      </c>
+      <c r="C23" t="s">
+        <v>49</v>
+      </c>
+      <c r="D23" t="s">
+        <v>146</v>
+      </c>
+      <c r="E23" s="3" t="n">
+        <v>0.0945886630561063</v>
+      </c>
+      <c r="F23" s="3" t="n">
+        <v>0.0087872490030933</v>
+      </c>
+      <c r="G23" s="3" t="n">
+        <v>-28.8455678365852</v>
+      </c>
+      <c r="H23" s="3" t="n">
+        <v>2.85472620329822</v>
+      </c>
+      <c r="I23" s="3" t="n">
+        <v>-26.1683537614787</v>
+      </c>
+      <c r="J23" s="3" t="n">
+        <v>2.67219127048893</v>
+      </c>
+      <c r="K23" s="3" t="n">
+        <v>0.905853802645135</v>
+      </c>
+      <c r="L23" s="3" t="n">
+        <v>0.00934053653817344</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>81</v>
+      </c>
+      <c r="B24" t="s">
+        <v>10</v>
+      </c>
+      <c r="C24" t="s">
+        <v>49</v>
+      </c>
+      <c r="D24" t="s">
+        <v>147</v>
+      </c>
+      <c r="E24" s="3" t="n">
+        <v>0.0938372244526644</v>
+      </c>
+      <c r="F24" s="3" t="n">
+        <v>0.0101736324235527</v>
+      </c>
+      <c r="G24" s="3" t="n">
+        <v>-26.6689613564787</v>
+      </c>
+      <c r="H24" s="3" t="n">
+        <v>0.311877900048043</v>
+      </c>
+      <c r="I24" s="3" t="n">
+        <v>-24.252141349137</v>
+      </c>
+      <c r="J24" s="3" t="n">
+        <v>0.958198885223177</v>
+      </c>
+      <c r="K24" s="3" t="n">
+        <v>0.905853802645135</v>
+      </c>
+      <c r="L24" s="3" t="n">
+        <v>0.00934053653817344</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>81</v>
+      </c>
+      <c r="B25" t="s">
+        <v>10</v>
+      </c>
+      <c r="C25" t="s">
+        <v>49</v>
+      </c>
+      <c r="D25" t="s">
+        <v>147</v>
+      </c>
+      <c r="E25" s="3" t="n">
+        <v>0.0876877703643507</v>
+      </c>
+      <c r="F25" s="3" t="n">
+        <v>0.0137146215924371</v>
+      </c>
+      <c r="G25" s="3" t="n">
+        <v>-26.5353063870661</v>
+      </c>
+      <c r="H25" s="3" t="n">
+        <v>0.743514413246525</v>
+      </c>
+      <c r="I25" s="3" t="n">
+        <v>-24.0283103795181</v>
+      </c>
+      <c r="J25" s="3" t="n">
+        <v>1.39608974156362</v>
+      </c>
+      <c r="K25" s="3" t="n">
+        <v>0.905853802645135</v>
+      </c>
+      <c r="L25" s="3" t="n">
+        <v>0.00934053653817344</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>81</v>
+      </c>
+      <c r="B26" t="s">
+        <v>10</v>
+      </c>
+      <c r="C26" t="s">
+        <v>49</v>
+      </c>
+      <c r="D26" t="s">
+        <v>147</v>
+      </c>
+      <c r="E26" s="3" t="n">
+        <v>0.0954068367677388</v>
+      </c>
+      <c r="F26" s="3" t="n">
+        <v>0.0144371119151015</v>
+      </c>
+      <c r="G26" s="3" t="n">
+        <v>-27.5239964709733</v>
+      </c>
+      <c r="H26" s="3" t="n">
+        <v>0.426560931293355</v>
+      </c>
+      <c r="I26" s="3" t="n">
+        <v>-23.6404969155835</v>
+      </c>
+      <c r="J26" s="3" t="n">
+        <v>0.956240684886901</v>
+      </c>
+      <c r="K26" s="3" t="n">
+        <v>0.905853802645135</v>
+      </c>
+      <c r="L26" s="3" t="n">
+        <v>0.00934053653817344</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>81</v>
+      </c>
+      <c r="B27" t="s">
+        <v>10</v>
+      </c>
+      <c r="C27" t="s">
+        <v>70</v>
+      </c>
+      <c r="D27" t="s">
+        <v>146</v>
+      </c>
+      <c r="E27" s="3" t="n">
+        <v>0.0928340665958652</v>
+      </c>
+      <c r="F27" s="3" t="n">
+        <v>0.0206860864282183</v>
+      </c>
+      <c r="G27" s="3" t="n">
+        <v>-26.1429492775033</v>
+      </c>
+      <c r="H27" s="3" t="n">
+        <v>0.311413050128636</v>
+      </c>
+      <c r="I27" s="3" t="n">
+        <v>-22.43363897761</v>
+      </c>
+      <c r="J27" s="3" t="n">
+        <v>1.23560127075556</v>
+      </c>
+      <c r="K27" s="3" t="n">
+        <v>0.847270404721274</v>
+      </c>
+      <c r="L27" s="3" t="n">
+        <v>0.0162504619702184</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>81</v>
+      </c>
+      <c r="B28" t="s">
+        <v>10</v>
+      </c>
+      <c r="C28" t="s">
+        <v>70</v>
+      </c>
+      <c r="D28" t="s">
+        <v>146</v>
+      </c>
+      <c r="E28" s="3" t="n">
+        <v>0.0697229619984634</v>
+      </c>
+      <c r="F28" s="3" t="n">
+        <v>0.0130662758837883</v>
+      </c>
+      <c r="G28" s="3" t="n">
+        <v>-24.6546190037421</v>
+      </c>
+      <c r="H28" s="3" t="n">
+        <v>0.503809178711708</v>
+      </c>
+      <c r="I28" s="3" t="n">
+        <v>-20.3981436017503</v>
+      </c>
+      <c r="J28" s="3" t="n">
+        <v>1.58518145565411</v>
+      </c>
+      <c r="K28" s="3" t="n">
+        <v>0.847270404721274</v>
+      </c>
+      <c r="L28" s="3" t="n">
+        <v>0.0162504619702184</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s">
+        <v>81</v>
+      </c>
+      <c r="B29" t="s">
+        <v>10</v>
+      </c>
+      <c r="C29" t="s">
+        <v>70</v>
+      </c>
+      <c r="D29" t="s">
+        <v>146</v>
+      </c>
+      <c r="E29" s="3" t="n">
+        <v>0.0803364088970866</v>
+      </c>
+      <c r="F29" s="3" t="n">
+        <v>0.0074534490338664</v>
+      </c>
+      <c r="G29" s="3" t="n">
+        <v>-23.789310404592</v>
+      </c>
+      <c r="H29" s="3" t="n">
+        <v>1.86074452816108</v>
+      </c>
+      <c r="I29" s="3" t="n">
+        <v>-20.4019918963007</v>
+      </c>
+      <c r="J29" s="3" t="n">
+        <v>0.721141804552036</v>
+      </c>
+      <c r="K29" s="3" t="n">
+        <v>0.847270404721274</v>
+      </c>
+      <c r="L29" s="3" t="n">
+        <v>0.0162504619702184</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s">
+        <v>104</v>
+      </c>
+      <c r="B30" t="s">
+        <v>38</v>
+      </c>
+      <c r="C30" t="s">
+        <v>49</v>
+      </c>
+      <c r="D30" t="s">
+        <v>146</v>
+      </c>
+      <c r="E30" s="3" t="n">
+        <v>0.456835254554257</v>
+      </c>
+      <c r="F30" s="3" t="n">
+        <v>0.202449890174201</v>
+      </c>
+      <c r="G30" s="3" t="n">
+        <v>-31.7841191112421</v>
+      </c>
+      <c r="H30" s="3" t="n">
+        <v>0.442733857547132</v>
+      </c>
+      <c r="I30" s="3" t="n">
+        <v>-15.3508900073733</v>
+      </c>
+      <c r="J30" s="3" t="n">
+        <v>0.384742441102943</v>
+      </c>
+      <c r="K30" s="3" t="n">
+        <v>0.487393975443699</v>
+      </c>
+      <c r="L30" s="3" t="n">
+        <v>0.00476070186935692</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s">
+        <v>104</v>
+      </c>
+      <c r="B31" t="s">
+        <v>38</v>
+      </c>
+      <c r="C31" t="s">
+        <v>49</v>
+      </c>
+      <c r="D31" t="s">
+        <v>146</v>
+      </c>
+      <c r="E31" s="3" t="n">
+        <v>0.413288403389533</v>
+      </c>
+      <c r="F31" s="3" t="n">
+        <v>0.112389945223684</v>
+      </c>
+      <c r="G31" s="3" t="n">
+        <v>-32.1772456511993</v>
+      </c>
+      <c r="H31" s="3" t="n">
+        <v>0.114888471204619</v>
+      </c>
+      <c r="I31" s="3" t="n">
+        <v>-15.3048234017503</v>
+      </c>
+      <c r="J31" s="3" t="n">
+        <v>0.0405687871269857</v>
+      </c>
+      <c r="K31" s="3" t="n">
+        <v>0.487393975443699</v>
+      </c>
+      <c r="L31" s="3" t="n">
+        <v>0.00476070186935692</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s">
+        <v>104</v>
+      </c>
+      <c r="B32" t="s">
+        <v>38</v>
+      </c>
+      <c r="C32" t="s">
+        <v>49</v>
+      </c>
+      <c r="D32" t="s">
+        <v>146</v>
+      </c>
+      <c r="E32" s="3" t="n">
+        <v>0.39097210965763</v>
+      </c>
+      <c r="F32" s="3" t="n">
+        <v>0.161614995604087</v>
+      </c>
+      <c r="G32" s="3" t="n">
+        <v>-33.7529221555991</v>
+      </c>
+      <c r="H32" s="3" t="n">
+        <v>2.40010318497478</v>
+      </c>
+      <c r="I32" s="3" t="n">
+        <v>-16.1457457850774</v>
+      </c>
+      <c r="J32" s="3" t="n">
+        <v>1.64199504031582</v>
+      </c>
+      <c r="K32" s="3" t="n">
+        <v>0.487393975443699</v>
+      </c>
+      <c r="L32" s="3" t="n">
+        <v>0.00476070186935692</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s">
+        <v>104</v>
+      </c>
+      <c r="B33" t="s">
+        <v>38</v>
+      </c>
+      <c r="C33" t="s">
+        <v>49</v>
+      </c>
+      <c r="D33" t="s">
+        <v>147</v>
+      </c>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
+      <c r="G33" s="3" t="n">
+        <v>-34.7241589378608</v>
+      </c>
+      <c r="H33" s="3" t="n">
+        <v>0.811832359880281</v>
+      </c>
+      <c r="I33" s="3" t="n">
+        <v>-17.3572679887203</v>
+      </c>
+      <c r="J33" s="3" t="n">
+        <v>0.192969119542348</v>
+      </c>
+      <c r="K33" s="3" t="n">
+        <v>0.487393975443699</v>
+      </c>
+      <c r="L33" s="3" t="n">
+        <v>0.00476070186935692</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s">
+        <v>104</v>
+      </c>
+      <c r="B34" t="s">
+        <v>38</v>
+      </c>
+      <c r="C34" t="s">
+        <v>49</v>
+      </c>
+      <c r="D34" t="s">
+        <v>147</v>
+      </c>
+      <c r="E34" s="3"/>
+      <c r="F34" s="3"/>
+      <c r="G34" s="3" t="n">
+        <v>-33.2085442064217</v>
+      </c>
+      <c r="H34" s="3" t="n">
+        <v>0.518919416124547</v>
+      </c>
+      <c r="I34" s="3" t="n">
+        <v>-15.74984207599</v>
+      </c>
+      <c r="J34" s="3" t="n">
+        <v>0.548761784549707</v>
+      </c>
+      <c r="K34" s="3" t="n">
+        <v>0.487393975443699</v>
+      </c>
+      <c r="L34" s="3" t="n">
+        <v>0.00476070186935692</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s">
+        <v>104</v>
+      </c>
+      <c r="B35" t="s">
+        <v>38</v>
+      </c>
+      <c r="C35" t="s">
+        <v>49</v>
+      </c>
+      <c r="D35" t="s">
+        <v>147</v>
+      </c>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3"/>
+      <c r="G35" s="3" t="n">
+        <v>-34.7716493996244</v>
+      </c>
+      <c r="H35" s="3" t="n">
+        <v>0.505351838454928</v>
+      </c>
+      <c r="I35" s="3" t="n">
+        <v>-17.5000491316568</v>
+      </c>
+      <c r="J35" s="3" t="n">
+        <v>0.157091965397041</v>
+      </c>
+      <c r="K35" s="3" t="n">
+        <v>0.487393975443699</v>
+      </c>
+      <c r="L35" s="3" t="n">
+        <v>0.00476070186935692</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s">
+        <v>121</v>
+      </c>
+      <c r="B36" t="s">
+        <v>48</v>
+      </c>
+      <c r="C36" t="s">
+        <v>122</v>
+      </c>
+      <c r="D36" t="s">
+        <v>146</v>
+      </c>
+      <c r="E36" s="3"/>
+      <c r="F36" s="3"/>
+      <c r="G36" s="3" t="n">
+        <v>-16.8890773598264</v>
+      </c>
+      <c r="H36" s="3" t="n">
+        <v>1.37501023265621</v>
+      </c>
+      <c r="I36" s="3" t="n">
+        <v>-15.6614793397953</v>
+      </c>
+      <c r="J36" s="3" t="n">
+        <v>1.23380376291122</v>
+      </c>
+      <c r="K36" s="3" t="n">
+        <v>0.915643588143238</v>
+      </c>
+      <c r="L36" s="3" t="n">
+        <v>0.00621994381504597</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="s">
+        <v>121</v>
+      </c>
+      <c r="B37" t="s">
+        <v>48</v>
+      </c>
+      <c r="C37" t="s">
+        <v>122</v>
+      </c>
+      <c r="D37" t="s">
+        <v>146</v>
+      </c>
+      <c r="E37" s="3" t="n">
+        <v>0.267505437513797</v>
+      </c>
+      <c r="F37" s="3" t="n">
+        <v>0.012340645572617</v>
+      </c>
+      <c r="G37" s="3" t="n">
+        <v>-16.67392350258</v>
+      </c>
+      <c r="H37" s="3" t="n">
+        <v>0.867126431146547</v>
+      </c>
+      <c r="I37" s="3" t="n">
+        <v>-15.4064434996604</v>
+      </c>
+      <c r="J37" s="3" t="n">
+        <v>0.673252399046126</v>
+      </c>
+      <c r="K37" s="3" t="n">
+        <v>0.915643588143238</v>
+      </c>
+      <c r="L37" s="3" t="n">
+        <v>0.00621994381504597</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="s">
+        <v>121</v>
+      </c>
+      <c r="B38" t="s">
+        <v>48</v>
+      </c>
+      <c r="C38" t="s">
+        <v>122</v>
+      </c>
+      <c r="D38" t="s">
+        <v>146</v>
+      </c>
+      <c r="E38" s="3" t="n">
+        <v>0.240695665525707</v>
+      </c>
+      <c r="F38" s="3" t="n">
+        <v>0.0239828377796496</v>
+      </c>
+      <c r="G38" s="3" t="n">
+        <v>-16.954550737517</v>
+      </c>
+      <c r="H38" s="3" t="n">
+        <v>0.619564311139797</v>
+      </c>
+      <c r="I38" s="3" t="n">
+        <v>-15.2603259331518</v>
+      </c>
+      <c r="J38" s="3" t="n">
+        <v>0.588900623640146</v>
+      </c>
+      <c r="K38" s="3" t="n">
+        <v>0.915643588143238</v>
+      </c>
+      <c r="L38" s="3" t="n">
+        <v>0.00621994381504597</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="s">
+        <v>132</v>
+      </c>
+      <c r="B39" t="s">
+        <v>38</v>
+      </c>
+      <c r="C39" t="s">
+        <v>133</v>
+      </c>
+      <c r="D39" t="s">
+        <v>146</v>
+      </c>
+      <c r="E39" s="3"/>
+      <c r="F39" s="3"/>
+      <c r="G39" s="3" t="n">
+        <v>-21.8266401005287</v>
+      </c>
+      <c r="H39" s="3" t="n">
+        <v>0.345377670352203</v>
+      </c>
+      <c r="I39" s="3" t="n">
+        <v>-12.2065310068627</v>
+      </c>
+      <c r="J39" s="3" t="n">
+        <v>0.425541418334075</v>
+      </c>
+      <c r="K39" s="3" t="n">
+        <v>0.546725559293581</v>
+      </c>
+      <c r="L39" s="3" t="n">
+        <v>0.010561206245293</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="s">
+        <v>132</v>
+      </c>
+      <c r="B40" t="s">
+        <v>38</v>
+      </c>
+      <c r="C40" t="s">
+        <v>133</v>
+      </c>
+      <c r="D40" t="s">
+        <v>146</v>
+      </c>
+      <c r="E40" s="3"/>
+      <c r="F40" s="3"/>
+      <c r="G40" s="3" t="n">
+        <v>-20.7682132916007</v>
+      </c>
+      <c r="H40" s="3" t="n">
+        <v>2.5569214656464</v>
+      </c>
+      <c r="I40" s="3" t="n">
+        <v>-11.6927700378924</v>
+      </c>
+      <c r="J40" s="3" t="n">
+        <v>0.178913224402233</v>
+      </c>
+      <c r="K40" s="3" t="n">
+        <v>0.546725559293581</v>
+      </c>
+      <c r="L40" s="3" t="n">
+        <v>0.010561206245293</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="E41" s="3"/>
+      <c r="F41" s="3"/>
+      <c r="G41" s="3"/>
+      <c r="H41" s="3"/>
+      <c r="I41" s="3"/>
+      <c r="J41" s="3"/>
+      <c r="K41" s="3"/>
+      <c r="L41" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>